<commit_message>
added comment , result
</commit_message>
<xml_diff>
--- a/Peace/condition.xlsx
+++ b/Peace/condition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\student\Peace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E382719-658E-45A2-A52D-6AED7B1CDCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B802A436-317B-4BB1-A827-F8A5C0AD10E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{62478793-8C76-4CF2-AE1E-E2F531C8A59E}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="398">
   <si>
     <t>ค่าใช้จ่าย Outsource</t>
   </si>
@@ -1149,9 +1149,6 @@
   </si>
   <si>
     <t>546017XX</t>
-  </si>
-  <si>
-    <t>6XXXXXXX</t>
   </si>
   <si>
     <t>51XXXXXX</t>
@@ -1630,7 +1627,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1639,7 +1636,7 @@
     <col min="2" max="2" width="49.85546875" customWidth="1"/>
     <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1657,10 +1654,10 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F1" t="s">
         <v>393</v>
-      </c>
-      <c r="F1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1674,7 +1671,7 @@
         <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1688,7 +1685,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1702,7 +1699,7 @@
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1716,7 +1713,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1730,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1744,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1761,43 +1758,43 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1811,7 +1808,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1825,29 +1822,29 @@
         <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C15" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1861,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1875,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1889,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1903,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1917,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1931,7 +1928,7 @@
         <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1945,7 +1942,7 @@
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1959,7 +1956,7 @@
         <v>43</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1973,18 +1970,18 @@
         <v>372</v>
       </c>
       <c r="E24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
-        <v>374</v>
+      <c r="A25" s="2">
+        <v>53601709</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add comment, add re for lowercase x
</commit_message>
<xml_diff>
--- a/Peace/condition.xlsx
+++ b/Peace/condition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\student\Peace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B802A436-317B-4BB1-A827-F8A5C0AD10E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C251BB-E769-48E8-92E3-382956C2C938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{62478793-8C76-4CF2-AE1E-E2F531C8A59E}"/>
   </bookViews>
@@ -122,9 +122,6 @@
     <t>ค่าสาธารณูปโภค</t>
   </si>
   <si>
-    <t>516017XX</t>
-  </si>
-  <si>
     <t>บันทึกรหัสกระบวนการทางธุรกิจ (กิจกรรม R, N, E)</t>
   </si>
   <si>
@@ -1221,6 +1218,9 @@
   </si>
   <si>
     <t>N0204$</t>
+  </si>
+  <si>
+    <t>516017xx</t>
   </si>
 </sst>
 </file>
@@ -1627,7 +1627,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1654,52 +1654,52 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F1" t="s">
         <v>392</v>
-      </c>
-      <c r="F1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1713,7 +1713,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1727,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1758,57 +1758,57 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1822,29 +1822,29 @@
         <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1858,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1872,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1886,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1900,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1914,63 +1914,63 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>40</v>
-      </c>
       <c r="E21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>42</v>
-      </c>
       <c r="E22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>372</v>
-      </c>
       <c r="E24" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1981,7 +1981,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2007,48 +2007,48 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" t="s">
         <v>151</v>
-      </c>
-      <c r="B1" t="s">
-        <v>152</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" t="s">
         <v>153</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>154</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>156</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>157</v>
-      </c>
-      <c r="K1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>160</v>
       </c>
-      <c r="C2" t="s">
-        <v>161</v>
-      </c>
       <c r="E2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" t="s">
         <v>162</v>
-      </c>
-      <c r="F2" t="s">
-        <v>163</v>
       </c>
       <c r="G2">
         <v>8101</v>
@@ -2057,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K2">
         <v>1000</v>
@@ -2065,19 +2065,19 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" t="s">
         <v>166</v>
       </c>
-      <c r="C3" t="s">
-        <v>167</v>
-      </c>
       <c r="E3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" t="s">
         <v>162</v>
-      </c>
-      <c r="F3" t="s">
-        <v>163</v>
       </c>
       <c r="G3">
         <v>8101</v>
@@ -2086,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K3">
         <v>1000</v>
@@ -2094,19 +2094,19 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" t="s">
         <v>169</v>
       </c>
-      <c r="C4" t="s">
-        <v>170</v>
-      </c>
       <c r="E4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" t="s">
         <v>162</v>
-      </c>
-      <c r="F4" t="s">
-        <v>163</v>
       </c>
       <c r="G4">
         <v>8101</v>
@@ -2115,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K4">
         <v>1000</v>
@@ -2123,19 +2123,19 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" t="s">
         <v>172</v>
       </c>
-      <c r="C5" t="s">
-        <v>173</v>
-      </c>
       <c r="E5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F5" t="s">
         <v>162</v>
-      </c>
-      <c r="F5" t="s">
-        <v>163</v>
       </c>
       <c r="G5">
         <v>8101</v>
@@ -2144,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K5">
         <v>1000</v>
@@ -2152,19 +2152,19 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" t="s">
         <v>175</v>
       </c>
-      <c r="C6" t="s">
-        <v>176</v>
-      </c>
       <c r="E6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" t="s">
         <v>162</v>
-      </c>
-      <c r="F6" t="s">
-        <v>163</v>
       </c>
       <c r="G6">
         <v>8101</v>
@@ -2173,7 +2173,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K6">
         <v>1000</v>
@@ -2181,19 +2181,19 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" t="s">
         <v>178</v>
       </c>
-      <c r="C7" t="s">
-        <v>179</v>
-      </c>
       <c r="E7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" t="s">
         <v>162</v>
-      </c>
-      <c r="F7" t="s">
-        <v>163</v>
       </c>
       <c r="G7">
         <v>8101</v>
@@ -2202,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K7">
         <v>1000</v>
@@ -2210,19 +2210,19 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" t="s">
         <v>181</v>
       </c>
-      <c r="C8" t="s">
-        <v>182</v>
-      </c>
       <c r="E8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" t="s">
         <v>162</v>
-      </c>
-      <c r="F8" t="s">
-        <v>163</v>
       </c>
       <c r="G8">
         <v>8101</v>
@@ -2231,7 +2231,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K8">
         <v>1000</v>
@@ -2239,19 +2239,19 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" t="s">
         <v>184</v>
       </c>
-      <c r="C9" t="s">
-        <v>185</v>
-      </c>
       <c r="E9" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" t="s">
         <v>162</v>
-      </c>
-      <c r="F9" t="s">
-        <v>163</v>
       </c>
       <c r="G9">
         <v>8101</v>
@@ -2260,7 +2260,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K9">
         <v>1000</v>
@@ -2268,19 +2268,19 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" t="s">
         <v>187</v>
       </c>
-      <c r="C10" t="s">
-        <v>188</v>
-      </c>
       <c r="E10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" t="s">
         <v>162</v>
-      </c>
-      <c r="F10" t="s">
-        <v>163</v>
       </c>
       <c r="G10">
         <v>8101</v>
@@ -2289,7 +2289,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K10">
         <v>1000</v>
@@ -2297,19 +2297,19 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" t="s">
         <v>190</v>
       </c>
-      <c r="C11" t="s">
-        <v>191</v>
-      </c>
       <c r="E11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F11" t="s">
         <v>162</v>
-      </c>
-      <c r="F11" t="s">
-        <v>163</v>
       </c>
       <c r="G11">
         <v>8101</v>
@@ -2318,7 +2318,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K11">
         <v>1000</v>
@@ -2326,19 +2326,19 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" t="s">
         <v>193</v>
       </c>
-      <c r="C12" t="s">
-        <v>194</v>
-      </c>
       <c r="E12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" t="s">
         <v>162</v>
-      </c>
-      <c r="F12" t="s">
-        <v>163</v>
       </c>
       <c r="G12">
         <v>8101</v>
@@ -2347,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K12">
         <v>1000</v>
@@ -2355,19 +2355,19 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" t="s">
         <v>196</v>
       </c>
-      <c r="C13" t="s">
-        <v>197</v>
-      </c>
       <c r="E13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" t="s">
         <v>162</v>
-      </c>
-      <c r="F13" t="s">
-        <v>163</v>
       </c>
       <c r="G13">
         <v>8101</v>
@@ -2376,7 +2376,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K13">
         <v>1000</v>
@@ -2384,19 +2384,19 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" t="s">
         <v>199</v>
       </c>
-      <c r="C14" t="s">
-        <v>200</v>
-      </c>
       <c r="E14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" t="s">
         <v>162</v>
-      </c>
-      <c r="F14" t="s">
-        <v>163</v>
       </c>
       <c r="G14">
         <v>8101</v>
@@ -2405,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K14">
         <v>1000</v>
@@ -2413,19 +2413,19 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" t="s">
         <v>202</v>
       </c>
-      <c r="C15" t="s">
-        <v>203</v>
-      </c>
       <c r="E15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F15" t="s">
         <v>162</v>
-      </c>
-      <c r="F15" t="s">
-        <v>163</v>
       </c>
       <c r="G15">
         <v>8101</v>
@@ -2434,7 +2434,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K15">
         <v>1000</v>
@@ -2442,19 +2442,19 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" t="s">
         <v>205</v>
       </c>
-      <c r="C16" t="s">
-        <v>206</v>
-      </c>
       <c r="E16" t="s">
+        <v>161</v>
+      </c>
+      <c r="F16" t="s">
         <v>162</v>
-      </c>
-      <c r="F16" t="s">
-        <v>163</v>
       </c>
       <c r="G16">
         <v>8101</v>
@@ -2463,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K16">
         <v>1000</v>
@@ -2471,19 +2471,19 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" t="s">
         <v>208</v>
       </c>
-      <c r="C17" t="s">
-        <v>209</v>
-      </c>
       <c r="E17" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17" t="s">
         <v>162</v>
-      </c>
-      <c r="F17" t="s">
-        <v>163</v>
       </c>
       <c r="G17">
         <v>8101</v>
@@ -2492,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K17">
         <v>1000</v>
@@ -2500,19 +2500,19 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" t="s">
         <v>211</v>
       </c>
-      <c r="C18" t="s">
-        <v>212</v>
-      </c>
       <c r="E18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F18" t="s">
         <v>162</v>
-      </c>
-      <c r="F18" t="s">
-        <v>163</v>
       </c>
       <c r="G18">
         <v>8101</v>
@@ -2521,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K18">
         <v>1000</v>
@@ -2529,19 +2529,19 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" t="s">
         <v>214</v>
       </c>
-      <c r="C19" t="s">
-        <v>215</v>
-      </c>
       <c r="E19" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" t="s">
         <v>162</v>
-      </c>
-      <c r="F19" t="s">
-        <v>163</v>
       </c>
       <c r="G19">
         <v>8101</v>
@@ -2550,7 +2550,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K19">
         <v>1000</v>
@@ -2558,19 +2558,19 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" t="s">
         <v>217</v>
       </c>
-      <c r="C20" t="s">
-        <v>218</v>
-      </c>
       <c r="E20" t="s">
+        <v>161</v>
+      </c>
+      <c r="F20" t="s">
         <v>162</v>
-      </c>
-      <c r="F20" t="s">
-        <v>163</v>
       </c>
       <c r="G20">
         <v>8101</v>
@@ -2579,7 +2579,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K20">
         <v>1000</v>
@@ -2587,19 +2587,19 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" t="s">
         <v>220</v>
       </c>
-      <c r="C21" t="s">
-        <v>221</v>
-      </c>
       <c r="E21" t="s">
+        <v>161</v>
+      </c>
+      <c r="F21" t="s">
         <v>162</v>
-      </c>
-      <c r="F21" t="s">
-        <v>163</v>
       </c>
       <c r="G21">
         <v>8101</v>
@@ -2608,7 +2608,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K21">
         <v>1000</v>
@@ -2616,19 +2616,19 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" t="s">
         <v>223</v>
       </c>
-      <c r="C22" t="s">
-        <v>224</v>
-      </c>
       <c r="E22" t="s">
+        <v>161</v>
+      </c>
+      <c r="F22" t="s">
         <v>162</v>
-      </c>
-      <c r="F22" t="s">
-        <v>163</v>
       </c>
       <c r="G22">
         <v>8101</v>
@@ -2637,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K22">
         <v>1000</v>
@@ -2645,19 +2645,19 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" t="s">
         <v>226</v>
       </c>
-      <c r="C23" t="s">
-        <v>227</v>
-      </c>
       <c r="E23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F23" t="s">
         <v>162</v>
-      </c>
-      <c r="F23" t="s">
-        <v>163</v>
       </c>
       <c r="G23">
         <v>8101</v>
@@ -2666,7 +2666,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K23">
         <v>1000</v>
@@ -2674,19 +2674,19 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" t="s">
         <v>229</v>
       </c>
-      <c r="C24" t="s">
-        <v>230</v>
-      </c>
       <c r="E24" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" t="s">
         <v>162</v>
-      </c>
-      <c r="F24" t="s">
-        <v>163</v>
       </c>
       <c r="G24">
         <v>8101</v>
@@ -2695,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K24">
         <v>1000</v>
@@ -2703,19 +2703,19 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" t="s">
         <v>232</v>
       </c>
-      <c r="C25" t="s">
-        <v>233</v>
-      </c>
       <c r="E25" t="s">
+        <v>161</v>
+      </c>
+      <c r="F25" t="s">
         <v>162</v>
-      </c>
-      <c r="F25" t="s">
-        <v>163</v>
       </c>
       <c r="G25">
         <v>8101</v>
@@ -2724,7 +2724,7 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K25">
         <v>1000</v>
@@ -2732,19 +2732,19 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" t="s">
         <v>235</v>
       </c>
-      <c r="C26" t="s">
-        <v>236</v>
-      </c>
       <c r="E26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" t="s">
         <v>162</v>
-      </c>
-      <c r="F26" t="s">
-        <v>163</v>
       </c>
       <c r="G26">
         <v>8101</v>
@@ -2753,7 +2753,7 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K26">
         <v>1000</v>
@@ -2761,19 +2761,19 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" t="s">
         <v>238</v>
       </c>
-      <c r="C27" t="s">
-        <v>239</v>
-      </c>
       <c r="E27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" t="s">
         <v>162</v>
-      </c>
-      <c r="F27" t="s">
-        <v>163</v>
       </c>
       <c r="G27">
         <v>8101</v>
@@ -2782,7 +2782,7 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K27">
         <v>1000</v>
@@ -2790,19 +2790,19 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" t="s">
         <v>241</v>
       </c>
-      <c r="C28" t="s">
-        <v>242</v>
-      </c>
       <c r="E28" t="s">
+        <v>161</v>
+      </c>
+      <c r="F28" t="s">
         <v>162</v>
-      </c>
-      <c r="F28" t="s">
-        <v>163</v>
       </c>
       <c r="G28">
         <v>8101</v>
@@ -2811,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K28">
         <v>1000</v>
@@ -2819,19 +2819,19 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" t="s">
         <v>244</v>
       </c>
-      <c r="C29" t="s">
-        <v>245</v>
-      </c>
       <c r="E29" t="s">
+        <v>161</v>
+      </c>
+      <c r="F29" t="s">
         <v>162</v>
-      </c>
-      <c r="F29" t="s">
-        <v>163</v>
       </c>
       <c r="G29">
         <v>8101</v>
@@ -2840,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K29">
         <v>1000</v>
@@ -2848,19 +2848,19 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" t="s">
         <v>247</v>
       </c>
-      <c r="C30" t="s">
-        <v>248</v>
-      </c>
       <c r="E30" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" t="s">
         <v>162</v>
-      </c>
-      <c r="F30" t="s">
-        <v>163</v>
       </c>
       <c r="G30">
         <v>8101</v>
@@ -2869,7 +2869,7 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K30">
         <v>1000</v>
@@ -2877,19 +2877,19 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="C31" t="s">
         <v>250</v>
       </c>
-      <c r="C31" t="s">
-        <v>251</v>
-      </c>
       <c r="E31" t="s">
+        <v>161</v>
+      </c>
+      <c r="F31" t="s">
         <v>162</v>
-      </c>
-      <c r="F31" t="s">
-        <v>163</v>
       </c>
       <c r="G31">
         <v>8101</v>
@@ -2898,7 +2898,7 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K31">
         <v>1000</v>
@@ -2906,19 +2906,19 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" t="s">
         <v>253</v>
       </c>
-      <c r="C32" t="s">
-        <v>254</v>
-      </c>
       <c r="E32" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" t="s">
         <v>162</v>
-      </c>
-      <c r="F32" t="s">
-        <v>163</v>
       </c>
       <c r="G32">
         <v>8101</v>
@@ -2927,7 +2927,7 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K32">
         <v>1000</v>
@@ -2935,19 +2935,19 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" t="s">
         <v>256</v>
       </c>
-      <c r="C33" t="s">
-        <v>257</v>
-      </c>
       <c r="E33" t="s">
+        <v>161</v>
+      </c>
+      <c r="F33" t="s">
         <v>162</v>
-      </c>
-      <c r="F33" t="s">
-        <v>163</v>
       </c>
       <c r="G33">
         <v>8101</v>
@@ -2956,7 +2956,7 @@
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K33">
         <v>1000</v>
@@ -2964,19 +2964,19 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" t="s">
         <v>259</v>
       </c>
-      <c r="C34" t="s">
-        <v>260</v>
-      </c>
       <c r="E34" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" t="s">
         <v>162</v>
-      </c>
-      <c r="F34" t="s">
-        <v>163</v>
       </c>
       <c r="G34">
         <v>8101</v>
@@ -2985,7 +2985,7 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K34">
         <v>1000</v>
@@ -2993,19 +2993,19 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C35" t="s">
         <v>262</v>
       </c>
-      <c r="C35" t="s">
-        <v>263</v>
-      </c>
       <c r="E35" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" t="s">
         <v>162</v>
-      </c>
-      <c r="F35" t="s">
-        <v>163</v>
       </c>
       <c r="G35">
         <v>8101</v>
@@ -3014,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K35">
         <v>1000</v>
@@ -3022,19 +3022,19 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="C36" t="s">
         <v>265</v>
       </c>
-      <c r="C36" t="s">
-        <v>266</v>
-      </c>
       <c r="E36" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" t="s">
         <v>162</v>
-      </c>
-      <c r="F36" t="s">
-        <v>163</v>
       </c>
       <c r="G36">
         <v>8101</v>
@@ -3043,7 +3043,7 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K36">
         <v>1000</v>
@@ -3051,19 +3051,19 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" t="s">
         <v>268</v>
       </c>
-      <c r="C37" t="s">
-        <v>269</v>
-      </c>
       <c r="E37" t="s">
+        <v>161</v>
+      </c>
+      <c r="F37" t="s">
         <v>162</v>
-      </c>
-      <c r="F37" t="s">
-        <v>163</v>
       </c>
       <c r="G37">
         <v>8101</v>
@@ -3072,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K37">
         <v>1000</v>
@@ -3080,19 +3080,19 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" t="s">
         <v>271</v>
       </c>
-      <c r="C38" t="s">
-        <v>272</v>
-      </c>
       <c r="E38" t="s">
+        <v>161</v>
+      </c>
+      <c r="F38" t="s">
         <v>162</v>
-      </c>
-      <c r="F38" t="s">
-        <v>163</v>
       </c>
       <c r="G38">
         <v>8101</v>
@@ -3101,7 +3101,7 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K38">
         <v>1000</v>
@@ -3109,19 +3109,19 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C39" t="s">
         <v>274</v>
       </c>
-      <c r="C39" t="s">
-        <v>275</v>
-      </c>
       <c r="E39" t="s">
+        <v>161</v>
+      </c>
+      <c r="F39" t="s">
         <v>162</v>
-      </c>
-      <c r="F39" t="s">
-        <v>163</v>
       </c>
       <c r="G39">
         <v>8101</v>
@@ -3130,7 +3130,7 @@
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K39">
         <v>1000</v>
@@ -3138,19 +3138,19 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
+        <v>275</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" t="s">
         <v>277</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40" t="s">
         <v>278</v>
-      </c>
-      <c r="E40" t="s">
-        <v>162</v>
-      </c>
-      <c r="F40" t="s">
-        <v>279</v>
       </c>
       <c r="G40">
         <v>8301</v>
@@ -3164,19 +3164,19 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C41" t="s">
+        <v>280</v>
+      </c>
+      <c r="E41" t="s">
+        <v>161</v>
+      </c>
+      <c r="F41" t="s">
         <v>281</v>
-      </c>
-      <c r="E41" t="s">
-        <v>162</v>
-      </c>
-      <c r="F41" t="s">
-        <v>282</v>
       </c>
       <c r="G41">
         <v>8301</v>
@@ -3190,19 +3190,19 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G42">
         <v>8301</v>
@@ -3216,19 +3216,19 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
+        <v>284</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C43" t="s">
         <v>286</v>
       </c>
-      <c r="C43" t="s">
+      <c r="E43" t="s">
+        <v>161</v>
+      </c>
+      <c r="F43" t="s">
         <v>287</v>
-      </c>
-      <c r="E43" t="s">
-        <v>162</v>
-      </c>
-      <c r="F43" t="s">
-        <v>288</v>
       </c>
       <c r="G43">
         <v>8301</v>
@@ -3242,19 +3242,19 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
+        <v>288</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="C44" t="s">
         <v>290</v>
       </c>
-      <c r="C44" t="s">
-        <v>291</v>
-      </c>
       <c r="E44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G44">
         <v>8301</v>
@@ -3268,19 +3268,19 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
+        <v>291</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="C45" t="s">
         <v>293</v>
       </c>
-      <c r="C45" t="s">
-        <v>294</v>
-      </c>
       <c r="E45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F45" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G45">
         <v>8301</v>
@@ -3294,19 +3294,19 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
+        <v>294</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="C46" t="s">
         <v>296</v>
       </c>
-      <c r="C46" t="s">
-        <v>297</v>
-      </c>
       <c r="E46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G46">
         <v>8301</v>
@@ -3320,19 +3320,19 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
+        <v>297</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="C47" t="s">
         <v>299</v>
       </c>
-      <c r="C47" t="s">
-        <v>300</v>
-      </c>
       <c r="E47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G47">
         <v>8301</v>
@@ -3346,19 +3346,19 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
+        <v>300</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="C48" t="s">
         <v>302</v>
       </c>
-      <c r="C48" t="s">
-        <v>303</v>
-      </c>
       <c r="E48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G48">
         <v>8301</v>
@@ -3372,19 +3372,19 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
+        <v>303</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="C49" t="s">
         <v>305</v>
       </c>
-      <c r="C49" t="s">
-        <v>306</v>
-      </c>
       <c r="E49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F49" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G49">
         <v>8301</v>
@@ -3398,19 +3398,19 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
+        <v>306</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="C50" t="s">
         <v>308</v>
       </c>
-      <c r="C50" t="s">
+      <c r="E50" t="s">
+        <v>161</v>
+      </c>
+      <c r="F50" t="s">
         <v>309</v>
-      </c>
-      <c r="E50" t="s">
-        <v>162</v>
-      </c>
-      <c r="F50" t="s">
-        <v>310</v>
       </c>
       <c r="G50">
         <v>8401</v>
@@ -3424,19 +3424,19 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
+        <v>310</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="C51" t="s">
         <v>312</v>
       </c>
-      <c r="C51" t="s">
-        <v>313</v>
-      </c>
       <c r="E51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F51" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G51">
         <v>8401</v>
@@ -3450,19 +3450,19 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
+        <v>313</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="C52" t="s">
         <v>315</v>
       </c>
-      <c r="C52" t="s">
-        <v>316</v>
-      </c>
       <c r="E52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F52" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G52">
         <v>8401</v>
@@ -3476,19 +3476,19 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
+        <v>316</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="C53" t="s">
         <v>318</v>
       </c>
-      <c r="C53" t="s">
-        <v>319</v>
-      </c>
       <c r="E53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F53" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G53">
         <v>8401</v>
@@ -3502,19 +3502,19 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
+        <v>319</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="C54" t="s">
         <v>321</v>
       </c>
-      <c r="C54" t="s">
-        <v>322</v>
-      </c>
       <c r="E54" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F54" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G54">
         <v>8401</v>
@@ -3528,19 +3528,19 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
+        <v>322</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="C55" t="s">
         <v>324</v>
       </c>
-      <c r="C55" t="s">
-        <v>325</v>
-      </c>
       <c r="E55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F55" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G55">
         <v>8401</v>
@@ -3554,19 +3554,19 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
+        <v>325</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="C56" t="s">
         <v>327</v>
       </c>
-      <c r="C56" t="s">
-        <v>328</v>
-      </c>
       <c r="E56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F56" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G56">
         <v>8401</v>
@@ -3580,19 +3580,19 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
+        <v>328</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="C57" t="s">
         <v>330</v>
       </c>
-      <c r="C57" t="s">
-        <v>331</v>
-      </c>
       <c r="E57" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F57" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G57">
         <v>8401</v>
@@ -3606,19 +3606,19 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" t="s">
+        <v>331</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="C58" t="s">
         <v>333</v>
       </c>
-      <c r="C58" t="s">
-        <v>334</v>
-      </c>
       <c r="E58" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F58" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G58">
         <v>8401</v>
@@ -3632,19 +3632,19 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
+        <v>334</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="C59" t="s">
         <v>336</v>
       </c>
-      <c r="C59" t="s">
-        <v>337</v>
-      </c>
       <c r="E59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F59" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G59">
         <v>8401</v>
@@ -3658,19 +3658,19 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
+        <v>337</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="C60" t="s">
         <v>339</v>
       </c>
-      <c r="C60" t="s">
-        <v>340</v>
-      </c>
       <c r="E60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F60" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G60">
         <v>8401</v>
@@ -3684,19 +3684,19 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
+        <v>340</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="C61" t="s">
         <v>342</v>
       </c>
-      <c r="C61" t="s">
-        <v>343</v>
-      </c>
       <c r="E61" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G61">
         <v>8401</v>
@@ -3710,19 +3710,19 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" t="s">
+        <v>343</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="C62" t="s">
         <v>345</v>
       </c>
-      <c r="C62" t="s">
-        <v>346</v>
-      </c>
       <c r="E62" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F62" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G62">
         <v>8401</v>
@@ -3736,19 +3736,19 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
+        <v>346</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="C63" t="s">
         <v>348</v>
       </c>
-      <c r="C63" t="s">
-        <v>349</v>
-      </c>
       <c r="E63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F63" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G63">
         <v>8401</v>
@@ -3762,19 +3762,19 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" t="s">
+        <v>349</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="C64" t="s">
         <v>351</v>
       </c>
-      <c r="C64" t="s">
-        <v>352</v>
-      </c>
       <c r="E64" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F64" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G64">
         <v>8401</v>
@@ -3788,19 +3788,19 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
+        <v>352</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="C65" t="s">
         <v>354</v>
       </c>
-      <c r="C65" t="s">
-        <v>355</v>
-      </c>
       <c r="E65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G65">
         <v>8401</v>
@@ -3814,19 +3814,19 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" t="s">
+        <v>355</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="C66" t="s">
         <v>357</v>
       </c>
-      <c r="C66" t="s">
-        <v>358</v>
-      </c>
       <c r="E66" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G66">
         <v>8401</v>
@@ -3840,19 +3840,19 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
+        <v>358</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="C67" t="s">
         <v>360</v>
       </c>
-      <c r="C67" t="s">
-        <v>361</v>
-      </c>
       <c r="E67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F67" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G67">
         <v>8401</v>
@@ -3866,19 +3866,19 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
+        <v>361</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="C68" t="s">
         <v>363</v>
       </c>
-      <c r="C68" t="s">
-        <v>364</v>
-      </c>
       <c r="E68" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F68" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G68">
         <v>8401</v>
@@ -3892,19 +3892,19 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
+        <v>364</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="C69" t="s">
         <v>366</v>
       </c>
-      <c r="C69" t="s">
-        <v>367</v>
-      </c>
       <c r="E69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F69" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G69">
         <v>8401</v>
@@ -3918,19 +3918,19 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
+        <v>367</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="C70" t="s">
         <v>369</v>
       </c>
-      <c r="C70" t="s">
-        <v>370</v>
-      </c>
       <c r="E70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F70" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G70">
         <v>8401</v>
@@ -3974,7 +3974,7 @@
         <v>101010001</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3982,7 +3982,7 @@
         <v>101010002</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3990,7 +3990,7 @@
         <v>101010004</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3998,7 +3998,7 @@
         <v>101010006</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4006,7 +4006,7 @@
         <v>101010009</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4014,7 +4014,7 @@
         <v>101010010</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4022,7 +4022,7 @@
         <v>101010012</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4030,7 +4030,7 @@
         <v>101010013</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4038,7 +4038,7 @@
         <v>101010015</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4046,7 +4046,7 @@
         <v>101010016</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4054,7 +4054,7 @@
         <v>101010019</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4062,7 +4062,7 @@
         <v>101014100</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4070,7 +4070,7 @@
         <v>101019901</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4078,7 +4078,7 @@
         <v>102010102</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4086,7 +4086,7 @@
         <v>102010103</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4094,7 +4094,7 @@
         <v>102010202</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4102,7 +4102,7 @@
         <v>102010205</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4110,7 +4110,7 @@
         <v>102010207</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4118,7 +4118,7 @@
         <v>102010301</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4126,7 +4126,7 @@
         <v>102010302</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4134,7 +4134,7 @@
         <v>102010408</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4142,7 +4142,7 @@
         <v>102014100</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4150,7 +4150,7 @@
         <v>102020006</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4158,7 +4158,7 @@
         <v>102020008</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4166,7 +4166,7 @@
         <v>102020016</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4174,7 +4174,7 @@
         <v>102024100</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4182,7 +4182,7 @@
         <v>102030010</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4190,7 +4190,7 @@
         <v>102030018</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4198,7 +4198,7 @@
         <v>102034100</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4206,7 +4206,7 @@
         <v>102039901</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4214,7 +4214,7 @@
         <v>103010002</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4222,7 +4222,7 @@
         <v>103010005</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4230,7 +4230,7 @@
         <v>103010006</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4238,7 +4238,7 @@
         <v>103010012</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -4246,7 +4246,7 @@
         <v>103010013</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4254,7 +4254,7 @@
         <v>103010019</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4262,7 +4262,7 @@
         <v>103010029</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4270,7 +4270,7 @@
         <v>103010032</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4278,7 +4278,7 @@
         <v>103010035</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -4286,7 +4286,7 @@
         <v>103010037</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -4294,7 +4294,7 @@
         <v>103014100</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -4302,7 +4302,7 @@
         <v>103019901</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4310,7 +4310,7 @@
         <v>103029901</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -4318,7 +4318,7 @@
         <v>104010014</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4326,7 +4326,7 @@
         <v>104010015</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -4334,7 +4334,7 @@
         <v>104010016</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -4342,7 +4342,7 @@
         <v>104010017</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4350,7 +4350,7 @@
         <v>104010018</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -4358,7 +4358,7 @@
         <v>104010019</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4366,7 +4366,7 @@
         <v>104010020</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4374,7 +4374,7 @@
         <v>104020001</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -4382,7 +4382,7 @@
         <v>104030001</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4390,7 +4390,7 @@
         <v>104070001</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4398,7 +4398,7 @@
         <v>104070002</v>
       </c>
       <c r="B55" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -4406,7 +4406,7 @@
         <v>104070003</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -4414,7 +4414,7 @@
         <v>104070004</v>
       </c>
       <c r="B57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -4422,7 +4422,7 @@
         <v>104080001</v>
       </c>
       <c r="B58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -4430,7 +4430,7 @@
         <v>104110002</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -4438,7 +4438,7 @@
         <v>104114100</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -4446,7 +4446,7 @@
         <v>181030003</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4454,7 +4454,7 @@
         <v>181039901</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -4462,7 +4462,7 @@
         <v>181050009</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4470,7 +4470,7 @@
         <v>181050010</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -4478,7 +4478,7 @@
         <v>181050011</v>
       </c>
       <c r="B65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -4486,7 +4486,7 @@
         <v>181060003</v>
       </c>
       <c r="B66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4494,7 +4494,7 @@
         <v>191010101</v>
       </c>
       <c r="B67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4502,7 +4502,7 @@
         <v>191010102</v>
       </c>
       <c r="B68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4510,7 +4510,7 @@
         <v>191010103</v>
       </c>
       <c r="B69" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -4518,7 +4518,7 @@
         <v>192020205</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -4526,7 +4526,7 @@
         <v>201010002</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4534,7 +4534,7 @@
         <v>201020002</v>
       </c>
       <c r="B72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -4542,7 +4542,7 @@
         <v>201040011</v>
       </c>
       <c r="B73" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -4550,7 +4550,7 @@
         <v>201040012</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -4558,7 +4558,7 @@
         <v>201040013</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -4566,7 +4566,7 @@
         <v>201040014</v>
       </c>
       <c r="B76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -4574,7 +4574,7 @@
         <v>201040016</v>
       </c>
       <c r="B77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -4582,7 +4582,7 @@
         <v>201040017</v>
       </c>
       <c r="B78" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -4590,7 +4590,7 @@
         <v>201040018</v>
       </c>
       <c r="B79" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -4598,7 +4598,7 @@
         <v>201040019</v>
       </c>
       <c r="B80" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -4606,7 +4606,7 @@
         <v>201040020</v>
       </c>
       <c r="B81" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -4614,7 +4614,7 @@
         <v>202030004</v>
       </c>
       <c r="B82" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -4622,7 +4622,7 @@
         <v>202050006</v>
       </c>
       <c r="B83" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -4630,7 +4630,7 @@
         <v>203030007</v>
       </c>
       <c r="B84" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -4638,7 +4638,7 @@
         <v>204020004</v>
       </c>
       <c r="B85" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -4646,7 +4646,7 @@
         <v>204020005</v>
       </c>
       <c r="B86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -4654,7 +4654,7 @@
         <v>204020006</v>
       </c>
       <c r="B87" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -4662,7 +4662,7 @@
         <v>204020007</v>
       </c>
       <c r="B88" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -4670,7 +4670,7 @@
         <v>204020009</v>
       </c>
       <c r="B89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -4678,7 +4678,7 @@
         <v>204020010</v>
       </c>
       <c r="B90" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -4686,7 +4686,7 @@
         <v>204020011</v>
       </c>
       <c r="B91" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -4694,7 +4694,7 @@
         <v>204020012</v>
       </c>
       <c r="B92" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -4702,7 +4702,7 @@
         <v>204030002</v>
       </c>
       <c r="B93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -4710,7 +4710,7 @@
         <v>204030003</v>
       </c>
       <c r="B94" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -4718,7 +4718,7 @@
         <v>204030006</v>
       </c>
       <c r="B95" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -4726,7 +4726,7 @@
         <v>204030008</v>
       </c>
       <c r="B96" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -4734,7 +4734,7 @@
         <v>204030015</v>
       </c>
       <c r="B97" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -4742,7 +4742,7 @@
         <v>204030018</v>
       </c>
       <c r="B98" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -4750,7 +4750,7 @@
         <v>204040001</v>
       </c>
       <c r="B99" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -4758,7 +4758,7 @@
         <v>204040003</v>
       </c>
       <c r="B100" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -4766,7 +4766,7 @@
         <v>204050001</v>
       </c>
       <c r="B101" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -4774,7 +4774,7 @@
         <v>204050002</v>
       </c>
       <c r="B102" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -4782,7 +4782,7 @@
         <v>204050003</v>
       </c>
       <c r="B103" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -4790,7 +4790,7 @@
         <v>204050004</v>
       </c>
       <c r="B104" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -4798,7 +4798,7 @@
         <v>204080001</v>
       </c>
       <c r="B105" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -4806,7 +4806,7 @@
         <v>204080002</v>
       </c>
       <c r="B106" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -4814,7 +4814,7 @@
         <v>205020002</v>
       </c>
       <c r="B107" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -4822,7 +4822,7 @@
         <v>205060002</v>
       </c>
       <c r="B108" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>